<commit_message>
pages with graphs and price prediction
</commit_message>
<xml_diff>
--- a/adresses.xlsx
+++ b/adresses.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nastasya Kirillovna\PycharmProjects\pythonProject2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danonchik/dev/anflat/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C34A86-AC6A-4142-AC18-9F289FB645FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="402">
   <si>
     <t>Широта</t>
   </si>
@@ -1222,12 +1223,15 @@
   </si>
   <si>
     <t>Рассказовка дер., Переделкино Ближнее мкр., кв-л 8, к. 1Б</t>
+  </si>
+  <si>
+    <t>Адрес</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1287,7 +1291,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1303,9 +1307,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1343,7 +1347,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1378,6 +1382,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1413,9 +1434,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1588,18 +1626,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D400"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="29.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B1" s="1">
-        <v>0</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1608,7 +1649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1622,7 +1663,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1636,7 +1677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1650,7 +1691,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1664,7 +1705,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1678,7 +1719,7 @@
         <v>36.272489999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1692,7 +1733,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1706,7 +1747,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1720,7 +1761,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1734,7 +1775,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1748,7 +1789,7 @@
         <v>37.738219999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1762,7 +1803,7 @@
         <v>37.442990000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1776,7 +1817,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1790,7 +1831,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1804,7 +1845,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1818,7 +1859,7 @@
         <v>37.485253</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1832,7 +1873,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1846,7 +1887,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1860,7 +1901,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1874,7 +1915,7 @@
         <v>37.503937999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1888,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1902,7 +1943,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1916,7 +1957,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1930,7 +1971,7 @@
         <v>37.198535999999997</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1944,7 +1985,7 @@
         <v>37.443986000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1958,7 +1999,7 @@
         <v>37.426890999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1972,7 +2013,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1986,7 +2027,7 @@
         <v>37.385528999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2000,7 +2041,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2014,7 +2055,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2028,7 +2069,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2042,7 +2083,7 @@
         <v>37.444538999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2056,7 +2097,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2070,7 +2111,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2084,7 +2125,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2098,7 +2139,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2112,7 +2153,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2126,7 +2167,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2140,7 +2181,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2154,7 +2195,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2168,7 +2209,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2182,7 +2223,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2196,7 +2237,7 @@
         <v>37.467457000000003</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2210,7 +2251,7 @@
         <v>37.377408000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2224,7 +2265,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2238,7 +2279,7 @@
         <v>37.354089000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2252,7 +2293,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2266,7 +2307,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2280,7 +2321,7 @@
         <v>37.327357999999997</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2294,7 +2335,7 @@
         <v>37.432220999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -2308,7 +2349,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2322,7 +2363,7 @@
         <v>37.494362000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2336,7 +2377,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2350,7 +2391,7 @@
         <v>37.494362000000002</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2364,7 +2405,7 @@
         <v>37.503937999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2378,7 +2419,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2392,7 +2433,7 @@
         <v>37.439266000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2406,7 +2447,7 @@
         <v>37.286057</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2420,7 +2461,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2434,7 +2475,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2448,7 +2489,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2462,7 +2503,7 @@
         <v>37.354089000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2476,7 +2517,7 @@
         <v>37.528584000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2490,7 +2531,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2504,7 +2545,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2518,7 +2559,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2532,7 +2573,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2546,7 +2587,7 @@
         <v>37.334752000000002</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2560,7 +2601,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2574,7 +2615,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2588,7 +2629,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2602,7 +2643,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2616,7 +2657,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2630,7 +2671,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2644,7 +2685,7 @@
         <v>37.443986000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2658,7 +2699,7 @@
         <v>37.334361000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2672,7 +2713,7 @@
         <v>37.479509999999998</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2686,7 +2727,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2700,7 +2741,7 @@
         <v>83.170685000000006</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2714,7 +2755,7 @@
         <v>37.508113000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2728,7 +2769,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2742,7 +2783,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2756,7 +2797,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2770,7 +2811,7 @@
         <v>37.103386</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2784,7 +2825,7 @@
         <v>37.472878000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2798,7 +2839,7 @@
         <v>37.467457000000003</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2812,7 +2853,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2826,7 +2867,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2840,7 +2881,7 @@
         <v>37.434824999999996</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2854,7 +2895,7 @@
         <v>37.323113999999997</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2868,7 +2909,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2882,7 +2923,7 @@
         <v>37.449350000000003</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2896,7 +2937,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2910,7 +2951,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2924,7 +2965,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2938,7 +2979,7 @@
         <v>37.376806999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2952,7 +2993,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2966,7 +3007,7 @@
         <v>37.470528999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -2980,7 +3021,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -2994,7 +3035,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3008,7 +3049,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3022,7 +3063,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3036,7 +3077,7 @@
         <v>37.418371999999998</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3050,7 +3091,7 @@
         <v>37.103386</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3064,7 +3105,7 @@
         <v>37.172801999999997</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3078,7 +3119,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3092,7 +3133,7 @@
         <v>37.453606000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3106,7 +3147,7 @@
         <v>37.443986000000002</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3120,7 +3161,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3134,7 +3175,7 @@
         <v>65.426154999999994</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3148,7 +3189,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3162,7 +3203,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3176,7 +3217,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3190,7 +3231,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3204,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3218,7 +3259,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3232,7 +3273,7 @@
         <v>37.103386</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3246,7 +3287,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3260,7 +3301,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3274,7 +3315,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3288,7 +3329,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3302,7 +3343,7 @@
         <v>37.286057</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3316,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3330,7 +3371,7 @@
         <v>73.394424999999998</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3344,7 +3385,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3358,7 +3399,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3372,7 +3413,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3386,7 +3427,7 @@
         <v>37.448537999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3400,7 +3441,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3414,7 +3455,7 @@
         <v>37.508113000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3428,7 +3469,7 @@
         <v>37.297260000000001</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3442,7 +3483,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3456,7 +3497,7 @@
         <v>37.494362000000002</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3470,7 +3511,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3484,7 +3525,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3498,7 +3539,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3512,7 +3553,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3526,7 +3567,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -3540,7 +3581,7 @@
         <v>37.508113000000002</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -3554,7 +3595,7 @@
         <v>37.453606000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -3568,7 +3609,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -3582,7 +3623,7 @@
         <v>37.503711000000003</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -3596,7 +3637,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -3610,7 +3651,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -3624,7 +3665,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -3638,7 +3679,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -3652,7 +3693,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -3666,7 +3707,7 @@
         <v>37.503711000000003</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -3680,7 +3721,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -3694,7 +3735,7 @@
         <v>65.425963999999993</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -3708,7 +3749,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -3722,7 +3763,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -3736,7 +3777,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -3750,7 +3791,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -3764,7 +3805,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -3778,7 +3819,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -3792,7 +3833,7 @@
         <v>37.385528999999998</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -3806,7 +3847,7 @@
         <v>37.487670000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -3820,7 +3861,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -3834,7 +3875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -3848,7 +3889,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -3862,7 +3903,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -3876,7 +3917,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -3890,7 +3931,7 @@
         <v>37.467457000000003</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -3904,7 +3945,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -3918,7 +3959,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -3932,7 +3973,7 @@
         <v>37.494362000000002</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -3946,7 +3987,7 @@
         <v>37.432220999999998</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -3960,7 +4001,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -3974,7 +4015,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -3988,7 +4029,7 @@
         <v>37.376806999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4002,7 +4043,7 @@
         <v>37.185046999999997</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4016,7 +4057,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -4030,7 +4071,7 @@
         <v>37.334752000000002</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -4044,7 +4085,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -4058,7 +4099,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -4072,7 +4113,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -4086,7 +4127,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -4100,7 +4141,7 @@
         <v>37.354089000000002</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -4114,7 +4155,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -4128,7 +4169,7 @@
         <v>37.473663000000002</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -4142,7 +4183,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -4156,7 +4197,7 @@
         <v>37.479509999999998</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -4170,7 +4211,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -4184,7 +4225,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -4198,7 +4239,7 @@
         <v>37.286057</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -4212,7 +4253,7 @@
         <v>37.326934999999999</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -4226,7 +4267,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -4240,7 +4281,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -4254,7 +4295,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -4268,7 +4309,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -4282,7 +4323,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -4296,7 +4337,7 @@
         <v>37.494362000000002</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -4310,7 +4351,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -4324,7 +4365,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -4338,7 +4379,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -4352,7 +4393,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -4366,7 +4407,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -4380,7 +4421,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -4394,7 +4435,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -4408,7 +4449,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -4422,7 +4463,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -4436,7 +4477,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -4450,7 +4491,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -4464,7 +4505,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -4478,7 +4519,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -4492,7 +4533,7 @@
         <v>37.385528999999998</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -4506,7 +4547,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -4520,7 +4561,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -4534,7 +4575,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -4548,7 +4589,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -4562,7 +4603,7 @@
         <v>37.183855000000001</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -4576,7 +4617,7 @@
         <v>37.528584000000002</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -4590,7 +4631,7 @@
         <v>37.475622000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -4604,7 +4645,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -4618,7 +4659,7 @@
         <v>83.170685000000006</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -4632,7 +4673,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -4646,7 +4687,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -4660,7 +4701,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -4674,7 +4715,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -4688,7 +4729,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -4702,7 +4743,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -4716,7 +4757,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -4730,7 +4771,7 @@
         <v>37.377408000000003</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -4744,7 +4785,7 @@
         <v>37.343449</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -4758,7 +4799,7 @@
         <v>37.326934999999999</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -4772,7 +4813,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -4786,7 +4827,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -4800,7 +4841,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -4814,7 +4855,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -4828,7 +4869,7 @@
         <v>37.376806999999999</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -4842,7 +4883,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -4856,7 +4897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -4870,7 +4911,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -4884,7 +4925,7 @@
         <v>37.436107</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -4898,7 +4939,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -4912,7 +4953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -4926,7 +4967,7 @@
         <v>37.442867999999997</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -4940,7 +4981,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -4954,7 +4995,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -4968,7 +5009,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -4982,7 +5023,7 @@
         <v>37.455016999999998</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -4996,7 +5037,7 @@
         <v>37.448537999999999</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -5010,7 +5051,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -5024,7 +5065,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -5038,7 +5079,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -5052,7 +5093,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -5066,7 +5107,7 @@
         <v>37.376806999999999</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -5080,7 +5121,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -5094,7 +5135,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -5108,7 +5149,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -5122,7 +5163,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -5136,7 +5177,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -5150,7 +5191,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -5164,7 +5205,7 @@
         <v>37.401802000000004</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -5178,7 +5219,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -5192,7 +5233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -5206,7 +5247,7 @@
         <v>37.350988999999998</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -5220,7 +5261,7 @@
         <v>37.376806999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -5234,7 +5275,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -5248,7 +5289,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -5262,7 +5303,7 @@
         <v>37.528584000000002</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -5276,7 +5317,7 @@
         <v>37.39152</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -5290,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -5304,7 +5345,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -5318,7 +5359,7 @@
         <v>37.503711000000003</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -5332,7 +5373,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -5346,7 +5387,7 @@
         <v>37.485605999999997</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -5360,7 +5401,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -5374,7 +5415,7 @@
         <v>37.494362000000002</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -5388,7 +5429,7 @@
         <v>37.432220999999998</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -5402,7 +5443,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="1">
         <v>271</v>
       </c>
@@ -5416,7 +5457,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274" s="1">
         <v>272</v>
       </c>
@@ -5430,7 +5471,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275" s="1">
         <v>273</v>
       </c>
@@ -5444,7 +5485,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276" s="1">
         <v>274</v>
       </c>
@@ -5458,7 +5499,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277" s="1">
         <v>275</v>
       </c>
@@ -5472,7 +5513,7 @@
         <v>37.467457000000003</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278" s="1">
         <v>276</v>
       </c>
@@ -5486,7 +5527,7 @@
         <v>37.448537999999999</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279" s="1">
         <v>277</v>
       </c>
@@ -5500,7 +5541,7 @@
         <v>37.334752000000002</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280" s="1">
         <v>278</v>
       </c>
@@ -5514,7 +5555,7 @@
         <v>37.351177</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281" s="1">
         <v>279</v>
       </c>
@@ -5528,7 +5569,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282" s="1">
         <v>280</v>
       </c>
@@ -5542,7 +5583,7 @@
         <v>37.473663000000002</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283" s="1">
         <v>281</v>
       </c>
@@ -5556,7 +5597,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284" s="1">
         <v>282</v>
       </c>
@@ -5570,7 +5611,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285" s="1">
         <v>283</v>
       </c>
@@ -5584,7 +5625,7 @@
         <v>37.475622000000001</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286" s="1">
         <v>284</v>
       </c>
@@ -5598,7 +5639,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287" s="1">
         <v>285</v>
       </c>
@@ -5612,7 +5653,7 @@
         <v>37.528584000000002</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288" s="1">
         <v>286</v>
       </c>
@@ -5626,7 +5667,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289" s="1">
         <v>287</v>
       </c>
@@ -5640,7 +5681,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290" s="1">
         <v>288</v>
       </c>
@@ -5654,7 +5695,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="1">
         <v>289</v>
       </c>
@@ -5668,7 +5709,7 @@
         <v>83.170685000000006</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292" s="1">
         <v>290</v>
       </c>
@@ -5682,7 +5723,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293" s="1">
         <v>291</v>
       </c>
@@ -5696,7 +5737,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294" s="1">
         <v>292</v>
       </c>
@@ -5710,7 +5751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295" s="1">
         <v>293</v>
       </c>
@@ -5724,7 +5765,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296" s="1">
         <v>294</v>
       </c>
@@ -5738,7 +5779,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297" s="1">
         <v>295</v>
       </c>
@@ -5752,7 +5793,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298" s="1">
         <v>296</v>
       </c>
@@ -5766,7 +5807,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299" s="1">
         <v>297</v>
       </c>
@@ -5780,7 +5821,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300" s="1">
         <v>298</v>
       </c>
@@ -5794,7 +5835,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301" s="1">
         <v>299</v>
       </c>
@@ -5808,7 +5849,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302" s="1">
         <v>300</v>
       </c>
@@ -5822,7 +5863,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303" s="1">
         <v>301</v>
       </c>
@@ -5836,7 +5877,7 @@
         <v>37.479717000000001</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304" s="1">
         <v>302</v>
       </c>
@@ -5850,7 +5891,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305" s="1">
         <v>303</v>
       </c>
@@ -5864,7 +5905,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306" s="1">
         <v>304</v>
       </c>
@@ -5878,7 +5919,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307" s="1">
         <v>305</v>
       </c>
@@ -5892,7 +5933,7 @@
         <v>37.323113999999997</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308" s="1">
         <v>306</v>
       </c>
@@ -5906,7 +5947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" s="1">
         <v>307</v>
       </c>
@@ -5920,7 +5961,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310" s="1">
         <v>308</v>
       </c>
@@ -5934,7 +5975,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311" s="1">
         <v>309</v>
       </c>
@@ -5948,7 +5989,7 @@
         <v>37.449350000000003</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312" s="1">
         <v>310</v>
       </c>
@@ -5962,7 +6003,7 @@
         <v>37.504097000000002</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313" s="1">
         <v>311</v>
       </c>
@@ -5976,7 +6017,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314" s="1">
         <v>312</v>
       </c>
@@ -5990,7 +6031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315" s="1">
         <v>313</v>
       </c>
@@ -6004,7 +6045,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316" s="1">
         <v>314</v>
       </c>
@@ -6018,7 +6059,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A317" s="1">
         <v>315</v>
       </c>
@@ -6032,7 +6073,7 @@
         <v>37.494467999999998</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A318" s="1">
         <v>316</v>
       </c>
@@ -6046,7 +6087,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A319" s="1">
         <v>317</v>
       </c>
@@ -6060,7 +6101,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A320" s="1">
         <v>318</v>
       </c>
@@ -6074,7 +6115,7 @@
         <v>37.528584000000002</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A321" s="1">
         <v>319</v>
       </c>
@@ -6088,7 +6129,7 @@
         <v>37.376806999999999</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A322" s="1">
         <v>320</v>
       </c>
@@ -6102,7 +6143,7 @@
         <v>37.449350000000003</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A323" s="1">
         <v>321</v>
       </c>
@@ -6116,7 +6157,7 @@
         <v>29.906659000000001</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A324" s="1">
         <v>322</v>
       </c>
@@ -6130,7 +6171,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A325" s="1">
         <v>323</v>
       </c>
@@ -6144,7 +6185,7 @@
         <v>63.141117999999999</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A326" s="1">
         <v>324</v>
       </c>
@@ -6158,7 +6199,7 @@
         <v>37.103386</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" s="1">
         <v>325</v>
       </c>
@@ -6172,7 +6213,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A328" s="1">
         <v>326</v>
       </c>
@@ -6186,7 +6227,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A329" s="1">
         <v>327</v>
       </c>
@@ -6200,7 +6241,7 @@
         <v>37.504097000000002</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A330" s="1">
         <v>328</v>
       </c>
@@ -6214,7 +6255,7 @@
         <v>37.370491000000001</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A331" s="1">
         <v>329</v>
       </c>
@@ -6228,7 +6269,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A332" s="1">
         <v>330</v>
       </c>
@@ -6242,7 +6283,7 @@
         <v>37.323113999999997</v>
       </c>
     </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A333" s="1">
         <v>331</v>
       </c>
@@ -6256,7 +6297,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A334" s="1">
         <v>332</v>
       </c>
@@ -6270,7 +6311,7 @@
         <v>37.185046999999997</v>
       </c>
     </row>
-    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A335" s="1">
         <v>333</v>
       </c>
@@ -6284,7 +6325,7 @@
         <v>37.385528999999998</v>
       </c>
     </row>
-    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A336" s="1">
         <v>334</v>
       </c>
@@ -6298,7 +6339,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A337" s="1">
         <v>335</v>
       </c>
@@ -6312,7 +6353,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A338" s="1">
         <v>336</v>
       </c>
@@ -6326,7 +6367,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A339" s="1">
         <v>337</v>
       </c>
@@ -6340,7 +6381,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A340" s="1">
         <v>338</v>
       </c>
@@ -6354,7 +6395,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A341" s="1">
         <v>339</v>
       </c>
@@ -6368,7 +6409,7 @@
         <v>37.487670000000001</v>
       </c>
     </row>
-    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A342" s="1">
         <v>340</v>
       </c>
@@ -6382,7 +6423,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A343" s="1">
         <v>341</v>
       </c>
@@ -6396,7 +6437,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A344" s="1">
         <v>342</v>
       </c>
@@ -6410,7 +6451,7 @@
         <v>37.470776000000001</v>
       </c>
     </row>
-    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345" s="1">
         <v>343</v>
       </c>
@@ -6424,7 +6465,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A346" s="1">
         <v>344</v>
       </c>
@@ -6438,7 +6479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A347" s="1">
         <v>345</v>
       </c>
@@ -6452,7 +6493,7 @@
         <v>37.286057</v>
       </c>
     </row>
-    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A348" s="1">
         <v>346</v>
       </c>
@@ -6466,7 +6507,7 @@
         <v>37.503711000000003</v>
       </c>
     </row>
-    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A349" s="1">
         <v>347</v>
       </c>
@@ -6480,7 +6521,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A350" s="1">
         <v>348</v>
       </c>
@@ -6494,7 +6535,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
         <v>349</v>
       </c>
@@ -6508,7 +6549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A352" s="1">
         <v>350</v>
       </c>
@@ -6522,7 +6563,7 @@
         <v>36.603960000000001</v>
       </c>
     </row>
-    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A353" s="1">
         <v>351</v>
       </c>
@@ -6536,7 +6577,7 @@
         <v>36.663294</v>
       </c>
     </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A354" s="1">
         <v>352</v>
       </c>
@@ -6550,7 +6591,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A355" s="1">
         <v>353</v>
       </c>
@@ -6564,7 +6605,7 @@
         <v>37.454754999999999</v>
       </c>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A356" s="1">
         <v>354</v>
       </c>
@@ -6578,7 +6619,7 @@
         <v>37.442990000000002</v>
       </c>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A357" s="1">
         <v>355</v>
       </c>
@@ -6592,7 +6633,7 @@
         <v>37.323563</v>
       </c>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A358" s="1">
         <v>356</v>
       </c>
@@ -6606,7 +6647,7 @@
         <v>37.286057</v>
       </c>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A359" s="1">
         <v>357</v>
       </c>
@@ -6620,7 +6661,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A360" s="1">
         <v>358</v>
       </c>
@@ -6634,7 +6675,7 @@
         <v>36.944446999999997</v>
       </c>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A361" s="1">
         <v>359</v>
       </c>
@@ -6648,7 +6689,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A362" s="1">
         <v>360</v>
       </c>
@@ -6662,7 +6703,7 @@
         <v>37.354089000000002</v>
       </c>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363" s="1">
         <v>361</v>
       </c>
@@ -6676,7 +6717,7 @@
         <v>37.325839999999999</v>
       </c>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A364" s="1">
         <v>362</v>
       </c>
@@ -6690,7 +6731,7 @@
         <v>37.354089000000002</v>
       </c>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A365" s="1">
         <v>363</v>
       </c>
@@ -6704,7 +6745,7 @@
         <v>37.477679999999999</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A366" s="1">
         <v>364</v>
       </c>
@@ -6718,7 +6759,7 @@
         <v>37.425735000000003</v>
       </c>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A367" s="1">
         <v>365</v>
       </c>
@@ -6732,7 +6773,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A368" s="1">
         <v>366</v>
       </c>
@@ -6746,7 +6787,7 @@
         <v>37.346136000000001</v>
       </c>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A369" s="1">
         <v>367</v>
       </c>
@@ -6760,7 +6801,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A370" s="1">
         <v>368</v>
       </c>
@@ -6774,7 +6815,7 @@
         <v>37.443103999999998</v>
       </c>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A371" s="1">
         <v>369</v>
       </c>
@@ -6788,7 +6829,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A372" s="1">
         <v>370</v>
       </c>
@@ -6802,7 +6843,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A373" s="1">
         <v>371</v>
       </c>
@@ -6816,7 +6857,7 @@
         <v>37.190314999999998</v>
       </c>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A374" s="1">
         <v>372</v>
       </c>
@@ -6830,7 +6871,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A375" s="1">
         <v>373</v>
       </c>
@@ -6844,7 +6885,7 @@
         <v>37.406410999999999</v>
       </c>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A376" s="1">
         <v>374</v>
       </c>
@@ -6858,7 +6899,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A377" s="1">
         <v>375</v>
       </c>
@@ -6872,7 +6913,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A378" s="1">
         <v>376</v>
       </c>
@@ -6886,7 +6927,7 @@
         <v>37.503081999999999</v>
       </c>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A379" s="1">
         <v>377</v>
       </c>
@@ -6900,7 +6941,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="380" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A380" s="1">
         <v>378</v>
       </c>
@@ -6914,7 +6955,7 @@
         <v>37.444538999999999</v>
       </c>
     </row>
-    <row r="381" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381" s="1">
         <v>379</v>
       </c>
@@ -6928,7 +6969,7 @@
         <v>36.917518999999999</v>
       </c>
     </row>
-    <row r="382" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A382" s="1">
         <v>380</v>
       </c>
@@ -6942,7 +6983,7 @@
         <v>37.495097000000001</v>
       </c>
     </row>
-    <row r="383" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A383" s="1">
         <v>381</v>
       </c>
@@ -6956,7 +6997,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="384" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A384" s="1">
         <v>382</v>
       </c>
@@ -6970,7 +7011,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="385" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A385" s="1">
         <v>383</v>
       </c>
@@ -6984,7 +7025,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="386" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A386" s="1">
         <v>384</v>
       </c>
@@ -6998,7 +7039,7 @@
         <v>37.572305999999998</v>
       </c>
     </row>
-    <row r="387" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A387" s="1">
         <v>385</v>
       </c>
@@ -7012,7 +7053,7 @@
         <v>37.424433000000001</v>
       </c>
     </row>
-    <row r="388" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A388" s="1">
         <v>386</v>
       </c>
@@ -7026,7 +7067,7 @@
         <v>37.432220999999998</v>
       </c>
     </row>
-    <row r="389" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A389" s="1">
         <v>387</v>
       </c>
@@ -7040,7 +7081,7 @@
         <v>37.441142999999997</v>
       </c>
     </row>
-    <row r="390" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A390" s="1">
         <v>388</v>
       </c>
@@ -7054,7 +7095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A391" s="1">
         <v>389</v>
       </c>
@@ -7068,7 +7109,7 @@
         <v>37.334752000000002</v>
       </c>
     </row>
-    <row r="392" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A392" s="1">
         <v>390</v>
       </c>
@@ -7082,7 +7123,7 @@
         <v>37.503711000000003</v>
       </c>
     </row>
-    <row r="393" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A393" s="1">
         <v>391</v>
       </c>
@@ -7096,7 +7137,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="394" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A394" s="1">
         <v>392</v>
       </c>
@@ -7110,7 +7151,7 @@
         <v>37.361660000000001</v>
       </c>
     </row>
-    <row r="395" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A395" s="1">
         <v>393</v>
       </c>
@@ -7124,7 +7165,7 @@
         <v>37.103386</v>
       </c>
     </row>
-    <row r="396" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A396" s="1">
         <v>394</v>
       </c>
@@ -7138,7 +7179,7 @@
         <v>37.477679999999999</v>
       </c>
     </row>
-    <row r="397" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A397" s="1">
         <v>395</v>
       </c>
@@ -7152,7 +7193,7 @@
         <v>37.491982</v>
       </c>
     </row>
-    <row r="398" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A398" s="1">
         <v>396</v>
       </c>
@@ -7166,7 +7207,7 @@
         <v>37.334752000000002</v>
       </c>
     </row>
-    <row r="399" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399" s="1">
         <v>397</v>
       </c>
@@ -7180,7 +7221,7 @@
         <v>37.481954000000002</v>
       </c>
     </row>
-    <row r="400" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A400" s="1">
         <v>398</v>
       </c>

</xml_diff>